<commit_message>
all Vlada text, table, and figure edits (except decision and projection tables
</commit_message>
<xml_diff>
--- a/report/tables/base_model_specs.xlsx
+++ b/report/tables/base_model_specs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sulca/Documents/Github/widow-assessment-update/report/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauricegoodman/Documents/widow-assessment-update/report/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A945F6D7-B922-1B44-B2BE-61BC2BB143F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366BE268-5E6B-444C-AB64-1B84D61C60C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" xr2:uid="{DEAB2F6C-895B-4DAD-9001-A1744A11A2B7}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t>Triennial survey timing</t>
   </si>
   <si>
-    <t>NWFSC WCGBT survey timing</t>
-  </si>
-  <si>
     <t>Fishing mortality methods</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
   </si>
   <si>
     <t>Triennial survey selectivity</t>
-  </si>
-  <si>
-    <t>NWFSC WCGBT survey selectivity</t>
   </si>
   <si>
     <t>Fishery time blocks</t>
@@ -181,6 +175,12 @@
   </si>
   <si>
     <t>HEAD</t>
+  </si>
+  <si>
+    <t>WCGBTS timing</t>
+  </si>
+  <si>
+    <t>WCGBTS selectivity</t>
   </si>
 </sst>
 </file>
@@ -559,7 +559,7 @@
   <dimension ref="B1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -569,7 +569,7 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
@@ -627,7 +627,7 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
@@ -693,7 +693,7 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F21">
         <v>0.65</v>
@@ -701,15 +701,15 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F23">
         <v>0.9</v>
@@ -717,103 +717,103 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="F29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="3:6" ht="32" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F35" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F36" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>